<commit_message>
tuple for button command=
</commit_message>
<xml_diff>
--- a/inventario.xlsx
+++ b/inventario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nombre</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>manzana</t>
-  </si>
-  <si>
-    <t>pera</t>
   </si>
   <si>
     <t>uva</t>
@@ -389,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,20 +419,9 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>1.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bug of utils
</commit_message>
<xml_diff>
--- a/inventario.xlsx
+++ b/inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,23 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>